<commit_message>
Commit after sharing updated draft with co-authors
</commit_message>
<xml_diff>
--- a/overall/Contrast Map.xlsx
+++ b/overall/Contrast Map.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs5_couples\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs5_couples\overall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6811F8E9-157F-4D1D-B336-7FD740B88B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFFF849-061C-43DA-9459-A8A67AA50E9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{3C24BD78-57BD-4508-BC48-48F0FE7C40B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="219">
   <si>
     <t>h_dm at w_ge40=0</t>
   </si>
@@ -544,6 +545,144 @@
   </si>
   <si>
     <t>Interaction of w_htn:religion_other</t>
+  </si>
+  <si>
+    <t>h_htn at both_general=0</t>
+  </si>
+  <si>
+    <t>h_htn at both_general=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_htn:both_general</t>
+  </si>
+  <si>
+    <t>w_htn at both_general=0</t>
+  </si>
+  <si>
+    <t>w_htn at both_general=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_htn:both_general</t>
+  </si>
+  <si>
+    <t>h_htn at both_obc=0</t>
+  </si>
+  <si>
+    <t>h_htn at both_obc=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_htn:both_obc</t>
+  </si>
+  <si>
+    <t>w_htn at both_obc=0</t>
+  </si>
+  <si>
+    <t>w_htn at both_obc=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_htn:both_obc</t>
+  </si>
+  <si>
+    <t>h_htn at both_scst=0</t>
+  </si>
+  <si>
+    <t>h_htn at both_scst=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_htn:both_scst</t>
+  </si>
+  <si>
+    <t>w_htn at both_scst=0</t>
+  </si>
+  <si>
+    <t>w_htn at both_scst=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_htn:both_scst</t>
+  </si>
+  <si>
+    <t>W6 General</t>
+  </si>
+  <si>
+    <t>H6 General</t>
+  </si>
+  <si>
+    <t>W6 OBC</t>
+  </si>
+  <si>
+    <t>H6 OBC</t>
+  </si>
+  <si>
+    <t>W6 SCST</t>
+  </si>
+  <si>
+    <t>H6 SCST</t>
+  </si>
+  <si>
+    <t>Caste: Both General</t>
+  </si>
+  <si>
+    <t>Caste: Both OBC</t>
+  </si>
+  <si>
+    <t>Caste: Both SCST</t>
+  </si>
+  <si>
+    <t>h_dm at both_general=0</t>
+  </si>
+  <si>
+    <t>h_dm at both_general=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_dm:both_general</t>
+  </si>
+  <si>
+    <t>w_dm at both_general=0</t>
+  </si>
+  <si>
+    <t>w_dm at both_general=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_dm:both_general</t>
+  </si>
+  <si>
+    <t>h_dm at both_obc=0</t>
+  </si>
+  <si>
+    <t>h_dm at both_obc=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_dm:both_obc</t>
+  </si>
+  <si>
+    <t>w_dm at both_obc=0</t>
+  </si>
+  <si>
+    <t>w_dm at both_obc=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_dm:both_obc</t>
+  </si>
+  <si>
+    <t>h_dm at both_scst=0</t>
+  </si>
+  <si>
+    <t>h_dm at both_scst=1</t>
+  </si>
+  <si>
+    <t>Interaction of h_dm:both_scst</t>
+  </si>
+  <si>
+    <t>w_dm at both_scst=0</t>
+  </si>
+  <si>
+    <t>w_dm at both_scst=1</t>
+  </si>
+  <si>
+    <t>Interaction of w_dm:both_scst</t>
+  </si>
+  <si>
+    <t>Caste: Intercaste</t>
   </si>
 </sst>
 </file>
@@ -895,15 +1034,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AC79E6-6A68-4A8B-9767-8407EBAB92FA}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1429,739 +1569,1090 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>100</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>203</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>192</v>
       </c>
       <c r="C59" t="s">
-        <v>100</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>204</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>205</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>207</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>102</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>210</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>211</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>213</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B80" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="C80" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C83" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B91" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B92" t="s">
-        <v>75</v>
-      </c>
-      <c r="C92" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C93" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
-      </c>
-      <c r="C95" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B96" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B97" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B98" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B100" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B104" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="C104" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C105" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="C107" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B109" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B110" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B111" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C111" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B112" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B114" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B115" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B116" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C117" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B118" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C120" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B122" t="s">
-        <v>81</v>
-      </c>
-      <c r="C122" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C123" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B124" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B125" t="s">
-        <v>82</v>
-      </c>
-      <c r="C125" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B126" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C126" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B127" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B128" t="s">
-        <v>83</v>
+        <v>191</v>
+      </c>
+      <c r="C128" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B129" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="C129" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B130" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>84</v>
+        <v>192</v>
+      </c>
+      <c r="C131" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B132" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="C132" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>178</v>
+      </c>
+      <c r="B133" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>179</v>
+      </c>
+      <c r="B134" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>180</v>
+      </c>
+      <c r="B135" t="s">
+        <v>193</v>
+      </c>
+      <c r="C135" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>181</v>
+      </c>
+      <c r="B136" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>182</v>
+      </c>
+      <c r="B137" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>183</v>
+      </c>
+      <c r="B138" t="s">
+        <v>194</v>
+      </c>
+      <c r="C138" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>184</v>
+      </c>
+      <c r="B139" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>185</v>
+      </c>
+      <c r="B140" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>186</v>
+      </c>
+      <c r="B141" t="s">
+        <v>195</v>
+      </c>
+      <c r="C141" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>187</v>
+      </c>
+      <c r="B142" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>188</v>
+      </c>
+      <c r="B143" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>189</v>
+      </c>
+      <c r="B144" t="s">
+        <v>196</v>
+      </c>
+      <c r="C144" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>190</v>
+      </c>
+      <c r="B145" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1F4238-C2CB-4BBC-AC17-EBECF4C6A259}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>172</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B24" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>